<commit_message>
modification d'une demande de congés
</commit_message>
<xml_diff>
--- a/media/excel_templates/evaluation_tmp.xlsx
+++ b/media/excel_templates/evaluation_tmp.xlsx
@@ -1082,7 +1082,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>Communication (rédaction de rapport)</t>
+          <t>Les problemes de la vie 2</t>
         </is>
       </c>
       <c r="C3" s="8" t="n"/>
@@ -1234,12 +1234,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bullock</t>
+          <t>Adam Young</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1247,12 +1247,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cameron</t>
+          <t>Allison Barnes</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Denise</t>
+          <t>Christina</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1260,12 +1260,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Duncan</t>
+          <t>Amanda Wilson</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Danielle</t>
+          <t>Andrew</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1273,12 +1273,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Christopher Adkins</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -1286,12 +1286,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lewis</t>
+          <t>David Thomas</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cindy</t>
+          <t>Jacob</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -1299,12 +1299,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Marks</t>
+          <t>Douglas Smith</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -1312,12 +1312,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Edward Rodriguez</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Joshua</t>
+          <t>Mason</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1325,12 +1325,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Patterson</t>
+          <t>Hurst</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -1338,12 +1338,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Matthew Mccarthy</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Donald</t>
+          <t>Sabrina</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -1351,15 +1351,132 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Matthew Pratt</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Alan</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Melton</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Jonathan</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Mr. Jeff Morgan</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Joshua</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Nicole Cooper</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Olivia</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Robinson</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Kelly</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Samantha Harris</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Kara</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Stacy Carlson MD</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Stephen Randolph</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Kathleen</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Steven Morales</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Rebecca</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>William Mckenzie</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Erika</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
fix maquette bugs and re-design etudiant create tuteur create
</commit_message>
<xml_diff>
--- a/media/excel_templates/evaluation_tmp.xlsx
+++ b/media/excel_templates/evaluation_tmp.xlsx
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>mat</t>
+          <t>devoir1</t>
         </is>
       </c>
       <c r="C3" s="8" t="n"/>
@@ -1234,12 +1234,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Carter</t>
+          <t>Armstrong</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rose</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1247,12 +1247,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>Bryant</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1260,12 +1260,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Gordon</t>
+          <t>Butler</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Timothy</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1273,12 +1273,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Harper</t>
+          <t>Carroll</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Teresa</t>
+          <t>Theresa</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -1286,12 +1286,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hawkins</t>
+          <t>Cross</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Lauren</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -1299,12 +1299,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Jarvis</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Deborah</t>
+          <t>Jesse</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -1312,12 +1312,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Kennedy</t>
+          <t>Hernandez</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1325,12 +1325,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Richards</t>
+          <t>Jensen</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -1338,12 +1338,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Kelly</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Tyler</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -1351,12 +1351,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Wilson</t>
+          <t>Schmitt</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Karen</t>
+          <t>William</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>

</xml_diff>

<commit_message>
modify evaluation student : show only active student to set not
</commit_message>
<xml_diff>
--- a/media/excel_templates/evaluation_tmp.xlsx
+++ b/media/excel_templates/evaluation_tmp.xlsx
@@ -1082,7 +1082,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>Communication (rédaction de rapport)</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="C3" s="8" t="n"/>
@@ -1234,132 +1234,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bullock</t>
+          <t>KONDI</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Abdoul Malik</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Cameron</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Denise</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Duncan</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Danielle</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Lee</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Brian</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Lewis</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Cindy</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Marks</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>David</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Murray</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Joshua</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Patterson</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Tammy</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Williams</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Donald</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Wright</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Alan</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>